<commit_message>
polity as a separate concept
</commit_message>
<xml_diff>
--- a/MaritimePiracy_Code/Codebook.xlsx
+++ b/MaritimePiracy_Code/Codebook.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
   <si>
     <t>Concept Label</t>
   </si>
@@ -237,6 +237,21 @@
   </si>
   <si>
     <t>continoues, squared</t>
+  </si>
+  <si>
+    <t>Polity</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Storm Dummy</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Earthquake Dummy</t>
   </si>
 </sst>
 </file>
@@ -585,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,38 +677,35 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
         <v>43</v>
@@ -701,159 +713,187 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>